<commit_message>
Correct datetime data in OpenRefine exports
</commit_message>
<xml_diff>
--- a/tests/bin/OpenRefine_exports/2_BR1_18-19.xlsx
+++ b/tests/bin/OpenRefine_exports/2_BR1_18-19.xlsx
@@ -168,7 +168,7 @@
         </is>
       </c>
       <c r="J2" s="1" t="n">
-        <v>43313.208333333336</v>
+        <v>43313.0</v>
       </c>
       <c r="K2" t="n">
         <v>2.0</v>
@@ -221,7 +221,7 @@
         </is>
       </c>
       <c r="J3" s="1" t="n">
-        <v>43344.208333333336</v>
+        <v>43344.0</v>
       </c>
       <c r="K3" t="n">
         <v>1.0</v>
@@ -274,7 +274,7 @@
         </is>
       </c>
       <c r="J4" s="1" t="n">
-        <v>43374.208333333336</v>
+        <v>43374.0</v>
       </c>
       <c r="K4" t="n">
         <v>2.0</v>
@@ -327,7 +327,7 @@
         </is>
       </c>
       <c r="J5" s="1" t="n">
-        <v>43405.208333333336</v>
+        <v>43405.0</v>
       </c>
       <c r="K5" t="n">
         <v>2.0</v>
@@ -380,7 +380,7 @@
         </is>
       </c>
       <c r="J6" s="1" t="n">
-        <v>43435.208333333336</v>
+        <v>43435.0</v>
       </c>
       <c r="K6" t="n">
         <v>3.0</v>
@@ -433,7 +433,7 @@
         </is>
       </c>
       <c r="J7" s="1" t="n">
-        <v>43466.208333333336</v>
+        <v>43466.0</v>
       </c>
       <c r="K7" t="n">
         <v>1.0</v>
@@ -486,7 +486,7 @@
         </is>
       </c>
       <c r="J8" s="1" t="n">
-        <v>43497.208333333336</v>
+        <v>43497.0</v>
       </c>
       <c r="K8" t="n">
         <v>3.0</v>
@@ -539,7 +539,7 @@
         </is>
       </c>
       <c r="J9" s="1" t="n">
-        <v>43525.208333333336</v>
+        <v>43525.0</v>
       </c>
       <c r="K9" t="n">
         <v>2.0</v>
@@ -592,7 +592,7 @@
         </is>
       </c>
       <c r="J10" s="1" t="n">
-        <v>43525.208333333336</v>
+        <v>43525.0</v>
       </c>
       <c r="K10" t="n">
         <v>1.0</v>

</xml_diff>